<commit_message>
updated the report and circuit
</commit_message>
<xml_diff>
--- a/Report/Project1Data.xlsx
+++ b/Report/Project1Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdjoh\Documents\GitHub\computer-architecture\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sleon\Documents\Git\computer-architecture\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5664"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="17250" windowHeight="5670"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>Input(s)</t>
   </si>
@@ -196,6 +196,63 @@
   </si>
   <si>
     <t>Long_Offset</t>
+  </si>
+  <si>
+    <t>Sign-Extend</t>
+  </si>
+  <si>
+    <t>ExceptionData</t>
+  </si>
+  <si>
+    <t>ExceptionFound</t>
+  </si>
+  <si>
+    <t>MemAddress</t>
+  </si>
+  <si>
+    <t>Read_Data</t>
+  </si>
+  <si>
+    <t>Data_Bus</t>
+  </si>
+  <si>
+    <t>PSW</t>
+  </si>
+  <si>
+    <t>PSW_P_IN</t>
+  </si>
+  <si>
+    <t>PSW_N_IN</t>
+  </si>
+  <si>
+    <t>PSW_Z_IN</t>
+  </si>
+  <si>
+    <t>PSW_P_OUT</t>
+  </si>
+  <si>
+    <t>PSW_N_OUT</t>
+  </si>
+  <si>
+    <t>PSW_Z_OUT</t>
+  </si>
+  <si>
+    <t>PSW_Overwrite</t>
+  </si>
+  <si>
+    <t>Privilaged_Clock</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>PCV</t>
+  </si>
+  <si>
+    <t>Timer_Overwrite</t>
   </si>
 </sst>
 </file>
@@ -628,30 +685,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E11"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3:AC15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>2</v>
       </c>
@@ -681,8 +746,24 @@
         <v>6</v>
       </c>
       <c r="Q1" s="11"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="11"/>
+      <c r="V1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="W1" s="11"/>
+      <c r="Y1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" s="11"/>
+      <c r="AB1" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC1" s="11"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -724,8 +805,32 @@
       <c r="Q2" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -753,16 +858,42 @@
       </c>
       <c r="L3" s="9"/>
       <c r="M3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="10"/>
+        <v>40</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="O3" s="9"/>
       <c r="P3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="Q3" s="10"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="10"/>
       <c r="C4" s="9"/>
@@ -785,13 +916,33 @@
         <v>49</v>
       </c>
       <c r="L4" s="9"/>
-      <c r="M4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="N4" s="10"/>
       <c r="O4" s="9"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="10"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="10"/>
+      <c r="Y4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC4" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="10"/>
       <c r="C5" s="9"/>
@@ -814,13 +965,33 @@
         <v>50</v>
       </c>
       <c r="L5" s="9"/>
-      <c r="M5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="N5" s="10"/>
       <c r="O5" s="9"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T5" s="10"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="10"/>
+      <c r="Y5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC5" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="10"/>
       <c r="C6" s="9"/>
@@ -837,13 +1008,29 @@
       <c r="J6" s="1"/>
       <c r="K6" s="10"/>
       <c r="L6" s="9"/>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="N6" s="10"/>
       <c r="O6" s="9"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S6" s="1"/>
+      <c r="T6" s="10"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="10"/>
+      <c r="Y6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z6" s="10"/>
+      <c r="AB6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC6" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="10"/>
       <c r="C7" s="9"/>
@@ -860,13 +1047,29 @@
       <c r="J7" s="1"/>
       <c r="K7" s="10"/>
       <c r="L7" s="9"/>
-      <c r="M7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="N7" s="10"/>
       <c r="O7" s="9"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="10"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S7" s="1"/>
+      <c r="T7" s="10"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="10"/>
+      <c r="Y7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z7" s="10"/>
+      <c r="AB7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC7" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="10"/>
       <c r="C8" s="9"/>
@@ -883,13 +1086,27 @@
       <c r="J8" s="1"/>
       <c r="K8" s="10"/>
       <c r="L8" s="9"/>
-      <c r="M8" s="1"/>
+      <c r="M8" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="N8" s="10"/>
       <c r="O8" s="9"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S8" s="1"/>
+      <c r="T8" s="10"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="10"/>
+      <c r="Y8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z8" s="10"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
@@ -911,8 +1128,18 @@
       <c r="O9" s="9"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="10"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S9" s="1"/>
+      <c r="T9" s="10"/>
+      <c r="Y9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z9" s="10"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="10"/>
       <c r="C10" s="9"/>
@@ -934,8 +1161,16 @@
       <c r="O10" s="9"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="10"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S10" s="1"/>
+      <c r="T10" s="10"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="10"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
@@ -957,8 +1192,16 @@
       <c r="O11" s="9"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="10"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S11" s="1"/>
+      <c r="T11" s="10"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="10"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="10"/>
       <c r="C12" s="9"/>
@@ -976,8 +1219,14 @@
       <c r="O12" s="9"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="10"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S12" s="1"/>
+      <c r="T12" s="10"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="10"/>
       <c r="C13" s="9"/>
@@ -995,8 +1244,14 @@
       <c r="O13" s="9"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="10"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S13" s="1"/>
+      <c r="T13" s="10"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="10"/>
       <c r="C14" s="9"/>
@@ -1014,8 +1269,14 @@
       <c r="O14" s="9"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="10"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S14" s="1"/>
+      <c r="T14" s="10"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="10"/>
       <c r="C15" s="9"/>
@@ -1033,8 +1294,14 @@
       <c r="O15" s="9"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S15" s="1"/>
+      <c r="T15" s="10"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="10"/>
       <c r="D16" s="1"/>
@@ -1048,8 +1315,12 @@
       <c r="N16" s="10"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="10"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S16" s="1"/>
+      <c r="T16" s="10"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="10"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="10"/>
       <c r="D17" s="1"/>
@@ -1062,8 +1333,12 @@
       <c r="N17" s="10"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="10"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S17" s="1"/>
+      <c r="T17" s="10"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="10"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="10"/>
       <c r="D18" s="1"/>
@@ -1076,8 +1351,12 @@
       <c r="N18" s="10"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="10"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S18" s="1"/>
+      <c r="T18" s="10"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="10"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="10"/>
       <c r="D19" s="1"/>
@@ -1090,8 +1369,10 @@
       <c r="N19" s="10"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="10"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S19" s="1"/>
+      <c r="T19" s="10"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="10"/>
       <c r="D20" s="1"/>
@@ -1104,9 +1385,15 @@
       <c r="N20" s="10"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="10"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
@@ -1115,6 +1402,7 @@
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1126,13 +1414,13 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1152,7 +1440,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1205,7 +1493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -1228,7 +1516,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1249,7 +1537,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1270,7 +1558,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -1291,7 +1579,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -1312,7 +1600,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -1333,7 +1621,7 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -1354,7 +1642,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1375,7 +1663,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -1396,7 +1684,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>